<commit_message>
se crea la hoja de embarque
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="PROCESO" sheetId="1" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>Agricultor</t>
   </si>
@@ -82,6 +82,9 @@
     <t>agricultor2</t>
   </si>
   <si>
+    <t>ANIBAL</t>
+  </si>
+  <si>
     <t>2014-09-23 11:48:27</t>
   </si>
   <si>
@@ -92,6 +95,78 @@
   </si>
   <si>
     <t>2014-10-03 15:51:48</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>Embarque</t>
+  </si>
+  <si>
+    <t>Fecha de entrega</t>
+  </si>
+  <si>
+    <t>Volumen</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Fletera</t>
+  </si>
+  <si>
+    <t>Chofer</t>
+  </si>
+  <si>
+    <t>Cel chofer</t>
+  </si>
+  <si>
+    <t>Fecha de arrivo</t>
+  </si>
+  <si>
+    <t>Destino</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Contacto de entrega</t>
+  </si>
+  <si>
+    <t>Chep</t>
+  </si>
+  <si>
+    <t>Ensenada</t>
+  </si>
+  <si>
+    <t>Tipo de ensenada</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Caja de transporte</t>
+  </si>
+  <si>
+    <t>Racks</t>
+  </si>
+  <si>
+    <t>22-09-2014</t>
+  </si>
+  <si>
+    <t>Trailer 53</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Retornable</t>
+  </si>
+  <si>
+    <t>Seca</t>
   </si>
 </sst>
 </file>
@@ -110,7 +185,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,14 +213,40 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6BBD44"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFe5e5e5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -156,6 +257,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="6" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -457,10 +564,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -578,15 +685,6 @@
       <c r="B4" s="3">
         <v>200000</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
@@ -595,15 +693,6 @@
       <c r="B5" s="3">
         <v>200000</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
@@ -612,15 +701,6 @@
       <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
@@ -629,15 +709,6 @@
       <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -646,15 +717,6 @@
       <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -663,15 +725,6 @@
       <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
@@ -706,19 +759,19 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2">
         <v>25000</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -733,34 +786,34 @@
         <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2">
         <v>25000</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2">
         <v>50000</v>
       </c>
       <c r="F13" s="2">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -772,7 +825,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -781,7 +834,7 @@
         <v>25000</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="2">
         <v>50000</v>
@@ -804,181 +857,127 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2">
+        <v>25000</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F15" s="2">
+        <v>50000</v>
+      </c>
+      <c r="G15" s="2">
+        <v>50000</v>
+      </c>
+      <c r="H15" s="2">
+        <v>50000</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>100</v>
+      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+        <v>200000</v>
+      </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>50000</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+        <v>200000</v>
+      </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
         <v>50000</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3">
         <v>50000</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="1" t="s">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2"/>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2">
         <v>10000</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
@@ -1005,133 +1004,145 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2">
         <v>10000</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="3">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="C27" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="B33" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1150,6 +1161,233 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20" customWidth="true" style="0"/>
+    <col min="4" max="4" width="30" customWidth="true" style="0"/>
+    <col min="5" max="5" width="20" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20" customWidth="true" style="0"/>
+    <col min="7" max="7" width="20" customWidth="true" style="0"/>
+    <col min="8" max="8" width="20" customWidth="true" style="0"/>
+    <col min="9" max="9" width="20" customWidth="true" style="0"/>
+    <col min="10" max="10" width="20" customWidth="true" style="0"/>
+    <col min="11" max="11" width="30" customWidth="true" style="0"/>
+    <col min="12" max="12" width="20" customWidth="true" style="0"/>
+    <col min="13" max="13" width="20" customWidth="true" style="0"/>
+    <col min="14" max="14" width="20" customWidth="true" style="0"/>
+    <col min="15" max="15" width="20" customWidth="true" style="0"/>
+    <col min="16" max="16" width="20" customWidth="true" style="0"/>
+    <col min="17" max="17" width="20" customWidth="true" style="0"/>
+    <col min="18" max="18" width="20" customWidth="true" style="0"/>
+    <col min="19" max="19" width="20" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="5">
+        <v>411</v>
+      </c>
+      <c r="B2" s="5">
+        <v>52</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5">
+        <v>50000</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="5">
+        <v>442</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="5">
+        <v>22</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1834</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="5">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5">
+        <v>10</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>10</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="5">
+        <v>411</v>
+      </c>
+      <c r="B3" s="5">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5">
+        <v>50000</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="5">
+        <v>442</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="5">
+        <v>22</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1834</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="5">
+        <v>10</v>
+      </c>
+      <c r="O3" s="5">
+        <v>10</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>10</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1175,32 +1413,4 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios en el ecxel
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -685,6 +685,15 @@
       <c r="B4" s="3">
         <v>200000</v>
       </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
@@ -693,6 +702,15 @@
       <c r="B5" s="3">
         <v>200000</v>
       </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
@@ -701,6 +719,15 @@
       <c r="B6" s="3">
         <v>0</v>
       </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
@@ -709,6 +736,15 @@
       <c r="B7" s="3">
         <v>0</v>
       </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -717,6 +753,15 @@
       <c r="B8" s="3">
         <v>0</v>
       </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -725,6 +770,15 @@
       <c r="B9" s="3">
         <v>0</v>
       </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
@@ -896,6 +950,15 @@
       <c r="B16" s="3">
         <v>200000</v>
       </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
@@ -904,6 +967,15 @@
       <c r="B17" s="3">
         <v>200000</v>
       </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
@@ -912,6 +984,15 @@
       <c r="B18" s="3">
         <v>50000</v>
       </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
@@ -920,6 +1001,15 @@
       <c r="B19" s="3">
         <v>50000</v>
       </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
@@ -928,12 +1018,30 @@
       <c r="B20" s="3">
         <v>50000</v>
       </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
@@ -1105,6 +1213,15 @@
       <c r="B28" s="3">
         <v>0</v>
       </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
@@ -1113,6 +1230,15 @@
       <c r="B29" s="3">
         <v>0</v>
       </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
@@ -1121,6 +1247,15 @@
       <c r="B30" s="3">
         <v>0</v>
       </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="3" t="s">
@@ -1129,6 +1264,15 @@
       <c r="B31" s="3">
         <v>0</v>
       </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
@@ -1137,12 +1281,30 @@
       <c r="B32" s="3">
         <v>0</v>
       </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1176,14 +1338,14 @@
     <col min="1" max="1" width="10" customWidth="true" style="0"/>
     <col min="2" max="2" width="20" customWidth="true" style="0"/>
     <col min="3" max="3" width="20" customWidth="true" style="0"/>
-    <col min="4" max="4" width="30" customWidth="true" style="0"/>
+    <col min="4" max="4" width="20" customWidth="true" style="0"/>
     <col min="5" max="5" width="20" customWidth="true" style="0"/>
     <col min="6" max="6" width="20" customWidth="true" style="0"/>
     <col min="7" max="7" width="20" customWidth="true" style="0"/>
     <col min="8" max="8" width="20" customWidth="true" style="0"/>
     <col min="9" max="9" width="20" customWidth="true" style="0"/>
     <col min="10" max="10" width="20" customWidth="true" style="0"/>
-    <col min="11" max="11" width="30" customWidth="true" style="0"/>
+    <col min="11" max="11" width="20" customWidth="true" style="0"/>
     <col min="12" max="12" width="20" customWidth="true" style="0"/>
     <col min="13" max="13" width="20" customWidth="true" style="0"/>
     <col min="14" max="14" width="20" customWidth="true" style="0"/>

</xml_diff>

<commit_message>
cambios en la tabla de excel
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -122,13 +122,13 @@
     <t>Fecha</t>
   </si>
   <si>
+    <t>Siembra</t>
+  </si>
+  <si>
+    <t>Germinacion</t>
+  </si>
+  <si>
     <t>Viabilidad</t>
-  </si>
-  <si>
-    <t>Siembra</t>
-  </si>
-  <si>
-    <t>Germinacion</t>
   </si>
   <si>
     <t>Injerto</t>
@@ -2202,11 +2202,11 @@
       <c r="D24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
@@ -2236,11 +2236,11 @@
       <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
@@ -2270,11 +2270,11 @@
       <c r="D26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
@@ -2304,11 +2304,11 @@
       <c r="D27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
se hacen cambios para poder agregar el alcance en la base de datos y en el excel
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -92,7 +92,10 @@
     <t>ENDEAVOR</t>
   </si>
   <si>
-    <t>29-09-2014</t>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>10-10-2014</t>
   </si>
   <si>
     <t>KAISER</t>
@@ -150,9 +153,6 @@
   </si>
   <si>
     <t>2014-09-22 14:31:24</t>
-  </si>
-  <si>
-    <t>100%</t>
   </si>
   <si>
     <t>Portainjerto</t>
@@ -1127,81 +1127,81 @@
         <v>23</v>
       </c>
       <c r="B14" s="2">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2">
+        <v>25000</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="2">
-        <v>50000</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="2">
+        <v>25000</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="2">
-        <v>50000</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2">
+        <v>25000</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="M14" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2">
+        <v>25000</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2">
-        <v>50000</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2">
+        <v>25000</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="2">
-        <v>50000</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2">
+        <v>25000</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="2">
-        <v>50000</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="2">
+        <v>25000</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="M15" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1339,7 +1339,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1426,7 +1426,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1513,7 +1513,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1641,7 +1641,7 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
@@ -1765,39 +1765,39 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -1806,7 +1806,7 @@
         <v>50000</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2">
         <v>100000</v>
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1844,7 +1844,7 @@
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2">
         <v>100000</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1925,39 +1925,39 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2028,12 +2028,12 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -2063,10 +2063,10 @@
         <v>50000</v>
       </c>
       <c r="K14" s="2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2074,7 +2074,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2">
         <v>25000</v>
@@ -2101,10 +2101,10 @@
         <v>50000</v>
       </c>
       <c r="K15" s="2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2151,7 +2151,9 @@
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>50000</v>
+      </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
@@ -2159,39 +2161,39 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -2259,7 +2261,7 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
@@ -2296,7 +2298,7 @@
         <v>45</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2">
         <v>10000</v>

</xml_diff>

<commit_message>
se modifican los archivos para incluir el scope en la bd
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -7,10 +7,11 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="DESGLOSE" sheetId="1" r:id="rId4"/>
-    <sheet name="PROCESO" sheetId="2" r:id="rId5"/>
-    <sheet name="EMBARQUE" sheetId="3" r:id="rId6"/>
-    <sheet name="CLIENTES" sheetId="4" r:id="rId7"/>
+    <sheet name="SEMILLAS" sheetId="1" r:id="rId4"/>
+    <sheet name="DESGLOSE" sheetId="2" r:id="rId5"/>
+    <sheet name="PROCESO" sheetId="3" r:id="rId6"/>
+    <sheet name="EMBARQUE" sheetId="4" r:id="rId7"/>
+    <sheet name="CLIENTES" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -18,11 +19,110 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>Agicultor</t>
+  </si>
+  <si>
+    <t>Semilla</t>
+  </si>
+  <si>
+    <t>Lote</t>
+  </si>
+  <si>
+    <t>Volumen</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Porcentaje de germinacion</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Cultivo</t>
+  </si>
   <si>
     <t>Agricultor</t>
   </si>
   <si>
+    <t>FORENZA</t>
+  </si>
+  <si>
+    <t>22-09-2014</t>
+  </si>
+  <si>
+    <t>Variedad</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>COLOSUS</t>
+  </si>
+  <si>
+    <t>DFGDFG</t>
+  </si>
+  <si>
+    <t>Portainjerto</t>
+  </si>
+  <si>
+    <t>Marca2</t>
+  </si>
+  <si>
+    <t>dfdf</t>
+  </si>
+  <si>
+    <t>07-10-2014</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>agricultor2</t>
+  </si>
+  <si>
+    <t>ENDEAVOR</t>
+  </si>
+  <si>
+    <t>lote</t>
+  </si>
+  <si>
+    <t>23-09-2014</t>
+  </si>
+  <si>
+    <t>marca</t>
+  </si>
+  <si>
+    <t>KAISER</t>
+  </si>
+  <si>
+    <t>ANIBAL</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>30-10-2014</t>
+  </si>
+  <si>
+    <t>23-10-2014</t>
+  </si>
+  <si>
     <t>FORENZA/COLOSUS</t>
   </si>
   <si>
@@ -65,42 +165,21 @@
     <t>FECHA DE TUTOREADO</t>
   </si>
   <si>
-    <t>FORENZA</t>
-  </si>
-  <si>
     <t>0%</t>
   </si>
   <si>
     <t>dd/mm/YY</t>
   </si>
   <si>
-    <t>COLOSUS</t>
-  </si>
-  <si>
-    <t>agricultor2</t>
-  </si>
-  <si>
     <t>ANIBAL/COLOSUS</t>
   </si>
   <si>
-    <t>ANIBAL</t>
-  </si>
-  <si>
     <t>ENDEAVOR/KAISER</t>
   </si>
   <si>
-    <t>ENDEAVOR</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
     <t>10-10-2014</t>
   </si>
   <si>
-    <t>KAISER</t>
-  </si>
-  <si>
     <t>ENDEAVOR/EMPOWER</t>
   </si>
   <si>
@@ -122,9 +201,6 @@
     <t>Pedido</t>
   </si>
   <si>
-    <t>Fecha</t>
-  </si>
-  <si>
     <t>Siembra</t>
   </si>
   <si>
@@ -149,15 +225,9 @@
     <t>Alcance</t>
   </si>
   <si>
-    <t>Variedad</t>
-  </si>
-  <si>
     <t>2014-09-22 14:31:24</t>
   </si>
   <si>
-    <t>Portainjerto</t>
-  </si>
-  <si>
     <t>TOTAL SEMBRADO</t>
   </si>
   <si>
@@ -182,21 +252,12 @@
     <t>2014-10-03 15:51:48</t>
   </si>
   <si>
-    <t>Orden</t>
-  </si>
-  <si>
-    <t>Agicultor</t>
-  </si>
-  <si>
     <t>Embarque</t>
   </si>
   <si>
     <t>Fecha de entrega</t>
   </si>
   <si>
-    <t>Volumen</t>
-  </si>
-  <si>
     <t>Transporte</t>
   </si>
   <si>
@@ -240,9 +301,6 @@
   </si>
   <si>
     <t>Racks</t>
-  </si>
-  <si>
-    <t>22-09-2014</t>
   </si>
   <si>
     <t>Trailer 53</t>
@@ -787,9 +845,338 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20" customWidth="true" style="0"/>
+    <col min="4" max="4" width="20" customWidth="true" style="0"/>
+    <col min="5" max="5" width="20" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20" customWidth="true" style="0"/>
+    <col min="7" max="7" width="20" customWidth="true" style="0"/>
+    <col min="8" max="8" width="20" customWidth="true" style="0"/>
+    <col min="9" max="9" width="20" customWidth="true" style="0"/>
+    <col min="10" max="10" width="20" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2">
+        <v>411</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2">
+        <v>411</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
+        <v>411</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
+        <v>411</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2">
+        <v>412</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
+        <v>412</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2">
+        <v>412</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2">
+        <v>412</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
@@ -812,913 +1199,913 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
         <v>25000</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2">
         <v>25000</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2">
         <v>25000</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="K14" s="2">
         <v>25000</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2">
         <v>25000</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2">
         <v>25000</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="H15" s="2">
         <v>25000</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="K15" s="2">
         <v>25000</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K29" s="2">
         <v>0</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1737,7 +2124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1761,52 +2148,52 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>50000</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E2" s="2">
         <v>100000</v>
@@ -1830,21 +2217,21 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2">
         <v>100000</v>
@@ -1868,12 +2255,12 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3">
         <v>200000</v>
@@ -1881,7 +2268,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3">
         <v>200000</v>
@@ -1889,7 +2276,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1897,7 +2284,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1905,7 +2292,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1913,7 +2300,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1921,52 +2308,52 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
         <v>25000</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2">
         <v>50000</v>
@@ -1990,21 +2377,21 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2">
         <v>25000</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2">
         <v>50000</v>
@@ -2028,21 +2415,21 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2">
         <v>25000</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2">
         <v>50000</v>
@@ -2066,21 +2453,21 @@
         <v>50000</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
         <v>25000</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2">
         <v>50000</v>
@@ -2104,12 +2491,12 @@
         <v>50000</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3">
         <v>200000</v>
@@ -2117,7 +2504,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B17" s="3">
         <v>200000</v>
@@ -2125,7 +2512,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3">
         <v>50000</v>
@@ -2133,7 +2520,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B19" s="3">
         <v>50000</v>
@@ -2141,7 +2528,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B20" s="3">
         <v>50000</v>
@@ -2149,7 +2536,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B21" s="3">
         <v>50000</v>
@@ -2157,52 +2544,52 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2">
         <v>10000</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2222,21 +2609,21 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="2">
         <v>10000</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2256,21 +2643,21 @@
         <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2">
         <v>10000</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2290,21 +2677,21 @@
         <v>0</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2">
         <v>10000</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2324,12 +2711,12 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -2337,7 +2724,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -2345,7 +2732,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="3" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -2353,7 +2740,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -2361,7 +2748,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -2369,7 +2756,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B33" s="3"/>
     </row>
@@ -2389,7 +2776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2425,64 +2812,64 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2490,34 +2877,34 @@
         <v>411</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>50000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I2" s="2">
         <v>442</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="L2" s="2">
         <v>22</v>
@@ -2526,7 +2913,7 @@
         <v>1834</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="O2" s="2">
         <v>10</v>
@@ -2535,13 +2922,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="R2" s="2">
         <v>10</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="T2" s="2">
         <v>10</v>
@@ -2552,34 +2939,34 @@
         <v>411</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2">
         <v>50000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I3" s="2">
         <v>442</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="L3" s="2">
         <v>22</v>
@@ -2588,7 +2975,7 @@
         <v>1834</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="O3" s="2">
         <v>10</v>
@@ -2597,13 +2984,13 @@
         <v>10</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="R3" s="2">
         <v>10</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="T3" s="2">
         <v>10</v>
@@ -2625,7 +3012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2653,51 +3040,51 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="F2" s="2">
         <v>7765434274</v>
@@ -2709,7 +3096,7 @@
         <v>7765434274</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="J2" s="2">
         <v>89203</v>
@@ -2717,19 +3104,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="F3" s="2">
         <v>101010</v>
@@ -2741,7 +3128,7 @@
         <v>101010</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="J3" s="2">
         <v>10101</v>
@@ -2749,19 +3136,19 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="F4" s="2">
         <v>6547801435</v>
@@ -2773,7 +3160,7 @@
         <v>6547801435</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="J4" s="2">
         <v>13456</v>
@@ -2781,13 +3168,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2795,28 +3182,28 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="G6" s="2">
         <v>442345632</v>
@@ -2825,7 +3212,7 @@
         <v>2145678</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="J6" s="2">
         <v>76988</v>
@@ -2833,19 +3220,19 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="F7" s="2">
         <v>6547890234</v>
@@ -2857,7 +3244,7 @@
         <v>6547890234</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="J7" s="2">
         <v>76456</v>
@@ -2865,19 +3252,19 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="F8" s="2">
         <v>5564523876</v>
@@ -2889,7 +3276,7 @@
         <v>5564523876</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="J8" s="2">
         <v>87654</v>

</xml_diff>

<commit_message>
condicional en consulta de generacion de excel
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
   <si>
     <t>Orden</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>23-10-2014</t>
+  </si>
+  <si>
+    <t>22-10-2014</t>
   </si>
   <si>
     <t>FORENZA/COLOSUS</t>
@@ -845,10 +848,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1150,6 +1153,38 @@
         <v>31</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
+        <v>413</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1204,48 +1239,48 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1256,37 +1291,37 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1297,37 +1332,37 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1337,48 +1372,48 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1389,37 +1424,37 @@
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1430,83 +1465,83 @@
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1520,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2">
         <v>25000</v>
@@ -1529,7 +1564,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H14" s="2">
         <v>25000</v>
@@ -1538,7 +1573,7 @@
         <v>14</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K14" s="2">
         <v>25000</v>
@@ -1547,7 +1582,7 @@
         <v>14</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1561,7 +1596,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2">
         <v>25000</v>
@@ -1570,7 +1605,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" s="2">
         <v>25000</v>
@@ -1579,7 +1614,7 @@
         <v>14</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K15" s="2">
         <v>25000</v>
@@ -1588,7 +1623,7 @@
         <v>14</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1598,48 +1633,48 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1650,37 +1685,37 @@
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1691,83 +1726,83 @@
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1778,293 +1813,293 @@
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K29" s="2">
         <v>0</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2075,37 +2110,37 @@
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2152,34 +2187,34 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2193,7 +2228,7 @@
         <v>50000</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2">
         <v>100000</v>
@@ -2231,7 +2266,7 @@
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2">
         <v>100000</v>
@@ -2260,7 +2295,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3">
         <v>200000</v>
@@ -2268,7 +2303,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3">
         <v>200000</v>
@@ -2276,7 +2311,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2284,7 +2319,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -2292,7 +2327,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2300,7 +2335,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2312,34 +2347,34 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2353,7 +2388,7 @@
         <v>25000</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2">
         <v>50000</v>
@@ -2391,7 +2426,7 @@
         <v>25000</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2">
         <v>50000</v>
@@ -2429,7 +2464,7 @@
         <v>25000</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2">
         <v>50000</v>
@@ -2467,7 +2502,7 @@
         <v>25000</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E15" s="2">
         <v>50000</v>
@@ -2496,7 +2531,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="3">
         <v>200000</v>
@@ -2504,7 +2539,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" s="3">
         <v>200000</v>
@@ -2512,7 +2547,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="3">
         <v>50000</v>
@@ -2520,7 +2555,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="3">
         <v>50000</v>
@@ -2528,7 +2563,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" s="3">
         <v>50000</v>
@@ -2536,7 +2571,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B21" s="3">
         <v>50000</v>
@@ -2548,34 +2583,34 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2589,7 +2624,7 @@
         <v>10000</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2609,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2623,7 +2658,7 @@
         <v>10000</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2643,7 +2678,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2657,7 +2692,7 @@
         <v>10000</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2677,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2691,7 +2726,7 @@
         <v>10000</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2711,12 +2746,12 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -2724,7 +2759,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -2732,7 +2767,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -2740,7 +2775,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -2748,7 +2783,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -2756,7 +2791,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B33" s="3"/>
     </row>
@@ -2818,58 +2853,58 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2889,13 +2924,13 @@
         <v>50000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I2" s="2">
         <v>442</v>
@@ -2904,7 +2939,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L2" s="2">
         <v>22</v>
@@ -2913,7 +2948,7 @@
         <v>1834</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O2" s="2">
         <v>10</v>
@@ -2922,13 +2957,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R2" s="2">
         <v>10</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T2" s="2">
         <v>10</v>
@@ -2951,13 +2986,13 @@
         <v>50000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2">
         <v>442</v>
@@ -2966,7 +3001,7 @@
         <v>12</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L3" s="2">
         <v>22</v>
@@ -2975,7 +3010,7 @@
         <v>1834</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O3" s="2">
         <v>10</v>
@@ -2984,13 +3019,13 @@
         <v>10</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R3" s="2">
         <v>10</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T3" s="2">
         <v>10</v>
@@ -3040,51 +3075,51 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" s="2">
         <v>7765434274</v>
@@ -3096,7 +3131,7 @@
         <v>7765434274</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J2" s="2">
         <v>89203</v>
@@ -3104,19 +3139,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F3" s="2">
         <v>101010</v>
@@ -3128,7 +3163,7 @@
         <v>101010</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J3" s="2">
         <v>10101</v>
@@ -3136,19 +3171,19 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F4" s="2">
         <v>6547801435</v>
@@ -3160,7 +3195,7 @@
         <v>6547801435</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J4" s="2">
         <v>13456</v>
@@ -3168,13 +3203,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -3182,28 +3217,28 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G6" s="2">
         <v>442345632</v>
@@ -3212,7 +3247,7 @@
         <v>2145678</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J6" s="2">
         <v>76988</v>
@@ -3220,19 +3255,19 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F7" s="2">
         <v>6547890234</v>
@@ -3244,7 +3279,7 @@
         <v>6547890234</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J7" s="2">
         <v>76456</v>
@@ -3252,19 +3287,19 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="2">
         <v>5564523876</v>
@@ -3276,7 +3311,7 @@
         <v>5564523876</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J8" s="2">
         <v>87654</v>

</xml_diff>

<commit_message>
se cambian de color los botones del usuario y se hace clickeable la informacion de la tabla para que todo diriga al informe
</commit_message>
<xml_diff>
--- a/reportes/reporte_plantanova.xlsx
+++ b/reportes/reporte_plantanova.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
   <si>
     <t>Orden</t>
   </si>
@@ -93,6 +93,15 @@
     <t>asd</t>
   </si>
   <si>
+    <t>dfdd</t>
+  </si>
+  <si>
+    <t>17-10-2014</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
     <t>agricultor2</t>
   </si>
   <si>
@@ -201,6 +210,9 @@
     <t>KENTON/KAISER</t>
   </si>
   <si>
+    <t>agri70000</t>
+  </si>
+  <si>
     <t>Pedido</t>
   </si>
   <si>
@@ -253,6 +265,9 @@
   </si>
   <si>
     <t>2014-10-03 15:51:48</t>
+  </si>
+  <si>
+    <t>2014-10-16 10:14:19</t>
   </si>
   <si>
     <t>Embarque</t>
@@ -848,10 +863,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1030,31 +1045,31 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2">
-        <v>50000</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5000</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>15</v>
@@ -1065,28 +1080,28 @@
         <v>412</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>50000</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
@@ -1097,22 +1112,22 @@
         <v>412</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2">
         <v>50000</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -1129,28 +1144,28 @@
         <v>412</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2">
         <v>50000</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>15</v>
@@ -1158,33 +1173,65 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2">
         <v>50000</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2">
+        <v>413</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1209,10 +1256,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1239,48 +1286,48 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1291,37 +1338,37 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1332,129 +1379,129 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1465,88 +1512,88 @@
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
         <v>25000</v>
@@ -1555,7 +1602,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2">
         <v>25000</v>
@@ -1564,7 +1611,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H14" s="2">
         <v>25000</v>
@@ -1573,7 +1620,7 @@
         <v>14</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K14" s="2">
         <v>25000</v>
@@ -1582,12 +1629,12 @@
         <v>14</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2">
         <v>25000</v>
@@ -1596,7 +1643,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2">
         <v>25000</v>
@@ -1605,7 +1652,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H15" s="2">
         <v>25000</v>
@@ -1614,7 +1661,7 @@
         <v>14</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K15" s="2">
         <v>25000</v>
@@ -1623,99 +1670,99 @@
         <v>14</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1726,421 +1773,554 @@
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K29" s="2">
         <v>0</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="L37" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K33" s="2">
-        <v>0</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>50</v>
+      <c r="M37" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" s="2">
+        <v>0</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2164,10 +2344,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2187,34 +2367,34 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2228,7 +2408,7 @@
         <v>50000</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E2" s="2">
         <v>100000</v>
@@ -2266,7 +2446,7 @@
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2">
         <v>100000</v>
@@ -2295,7 +2475,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3">
         <v>200000</v>
@@ -2303,7 +2483,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B5" s="3">
         <v>200000</v>
@@ -2311,7 +2491,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2319,7 +2499,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -2327,7 +2507,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2335,7 +2515,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2343,38 +2523,38 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2382,13 +2562,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2">
         <v>25000</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E12" s="2">
         <v>50000</v>
@@ -2426,7 +2606,7 @@
         <v>25000</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E13" s="2">
         <v>50000</v>
@@ -2458,13 +2638,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
         <v>25000</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E14" s="2">
         <v>50000</v>
@@ -2496,13 +2676,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2">
         <v>25000</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2">
         <v>50000</v>
@@ -2531,7 +2711,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B16" s="3">
         <v>200000</v>
@@ -2539,7 +2719,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B17" s="3">
         <v>200000</v>
@@ -2547,7 +2727,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B18" s="3">
         <v>50000</v>
@@ -2555,7 +2735,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B19" s="3">
         <v>50000</v>
@@ -2563,7 +2743,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B20" s="3">
         <v>50000</v>
@@ -2571,7 +2751,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B21" s="3">
         <v>50000</v>
@@ -2579,38 +2759,38 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2618,13 +2798,13 @@
         <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2">
         <v>10000</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2644,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2658,7 +2838,7 @@
         <v>10000</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2678,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2686,13 +2866,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2">
         <v>10000</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2712,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2720,13 +2900,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
         <v>10000</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2746,12 +2926,12 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -2759,7 +2939,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -2767,7 +2947,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -2775,7 +2955,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -2783,7 +2963,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -2791,9 +2971,125 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="2">
+        <v>70000</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -2853,58 +3149,58 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2924,13 +3220,13 @@
         <v>50000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I2" s="2">
         <v>442</v>
@@ -2939,7 +3235,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L2" s="2">
         <v>22</v>
@@ -2948,7 +3244,7 @@
         <v>1834</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="O2" s="2">
         <v>10</v>
@@ -2957,13 +3253,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="R2" s="2">
         <v>10</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="T2" s="2">
         <v>10</v>
@@ -2986,13 +3282,13 @@
         <v>50000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I3" s="2">
         <v>442</v>
@@ -3001,7 +3297,7 @@
         <v>12</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L3" s="2">
         <v>22</v>
@@ -3010,7 +3306,7 @@
         <v>1834</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="O3" s="2">
         <v>10</v>
@@ -3019,13 +3315,13 @@
         <v>10</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="R3" s="2">
         <v>10</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="T3" s="2">
         <v>10</v>
@@ -3075,51 +3371,51 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2">
         <v>7765434274</v>
@@ -3131,7 +3427,7 @@
         <v>7765434274</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="J2" s="2">
         <v>89203</v>
@@ -3139,19 +3435,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F3" s="2">
         <v>101010</v>
@@ -3163,7 +3459,7 @@
         <v>101010</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="J3" s="2">
         <v>10101</v>
@@ -3171,19 +3467,19 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2">
         <v>6547801435</v>
@@ -3195,7 +3491,7 @@
         <v>6547801435</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="J4" s="2">
         <v>13456</v>
@@ -3203,13 +3499,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -3217,28 +3513,28 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G6" s="2">
         <v>442345632</v>
@@ -3247,7 +3543,7 @@
         <v>2145678</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J6" s="2">
         <v>76988</v>
@@ -3255,19 +3551,19 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F7" s="2">
         <v>6547890234</v>
@@ -3279,7 +3575,7 @@
         <v>6547890234</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="J7" s="2">
         <v>76456</v>
@@ -3287,19 +3583,19 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F8" s="2">
         <v>5564523876</v>
@@ -3311,7 +3607,7 @@
         <v>5564523876</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="J8" s="2">
         <v>87654</v>

</xml_diff>